<commit_message>
upload dr merve's annotated + created 3 trials for standard deviation
</commit_message>
<xml_diff>
--- a/dataset/annotations2/mandible measurement.xlsx
+++ b/dataset/annotations2/mandible measurement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Masaüstü\ai mandible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7833f654840b5b66/Masaüstü/ai mandible/annotated and non-annotated mandible X-rays and measurement results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7D2C5B-2F50-481E-A51B-462507B7DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{F39315D2-F34B-4326-A5BA-CB47F1D79398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{700EA80D-7597-4476-A396-5C2A74FC8995}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10980" windowHeight="10080" xr2:uid="{2A870678-B445-4109-BF97-6723C2B031AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2A870678-B445-4109-BF97-6723C2B031AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Case Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -129,6 +126,99 @@
   </si>
   <si>
     <t>#1405973</t>
+  </si>
+  <si>
+    <t>#1506536</t>
+  </si>
+  <si>
+    <t>#1506343</t>
+  </si>
+  <si>
+    <t>#1409435</t>
+  </si>
+  <si>
+    <t>#1507529</t>
+  </si>
+  <si>
+    <t>#1503378</t>
+  </si>
+  <si>
+    <t>#1509616</t>
+  </si>
+  <si>
+    <t>#1509982</t>
+  </si>
+  <si>
+    <t>#1509479</t>
+  </si>
+  <si>
+    <t>#1508098</t>
+  </si>
+  <si>
+    <t>#1508936</t>
+  </si>
+  <si>
+    <t>#1510422</t>
+  </si>
+  <si>
+    <t>#1512125</t>
+  </si>
+  <si>
+    <t>#1510921</t>
+  </si>
+  <si>
+    <t>#1510985</t>
+  </si>
+  <si>
+    <t>#1510906</t>
+  </si>
+  <si>
+    <t>#1510488</t>
+  </si>
+  <si>
+    <t>#1513314</t>
+  </si>
+  <si>
+    <t>#1513522</t>
+  </si>
+  <si>
+    <t>#1512246</t>
+  </si>
+  <si>
+    <t>#1513551</t>
+  </si>
+  <si>
+    <t>#1513682</t>
+  </si>
+  <si>
+    <t>#1514519</t>
+  </si>
+  <si>
+    <t>#1514834</t>
+  </si>
+  <si>
+    <t>#1517089</t>
+  </si>
+  <si>
+    <t>#1518809</t>
+  </si>
+  <si>
+    <t>#1516578</t>
+  </si>
+  <si>
+    <t>#1521723</t>
+  </si>
+  <si>
+    <t>#1521480</t>
+  </si>
+  <si>
+    <t>#1520943</t>
+  </si>
+  <si>
+    <t>X-ray Number</t>
+  </si>
+  <si>
+    <t>#1519932</t>
   </si>
 </sst>
 </file>
@@ -172,9 +262,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,6 +282,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,34 +585,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118929CC-1E83-46F5-AB1A-F7177A411D1A}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>40.07</v>
@@ -532,8 +631,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>12.15</v>
@@ -549,8 +648,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>18.86</v>
@@ -566,8 +665,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>16.04</v>
@@ -583,8 +682,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B6">
         <v>18.53</v>
@@ -600,8 +699,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
+      <c r="A7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B7">
         <v>19.04</v>
@@ -617,8 +716,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
+      <c r="A8" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B8">
         <v>13.03</v>
@@ -646,8 +745,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
+      <c r="A9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B9">
         <v>16.97</v>
@@ -675,8 +774,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
+      <c r="A10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B10">
         <v>13.36</v>
@@ -704,8 +803,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
+      <c r="A11" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B11">
         <v>19.21</v>
@@ -733,8 +832,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>15</v>
+      <c r="A12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B12">
         <v>22.34</v>
@@ -762,8 +861,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
+      <c r="A13" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B13">
         <v>13.39</v>
@@ -791,8 +890,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
+      <c r="A14" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B14">
         <v>14.63</v>
@@ -820,8 +919,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
+      <c r="A15" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B15">
         <v>20.64</v>
@@ -849,8 +948,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>19</v>
+      <c r="A16" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B16">
         <v>21.98</v>
@@ -877,9 +976,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>20</v>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B17">
         <v>18.22</v>
@@ -894,9 +993,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B18">
         <v>16.149999999999999</v>
@@ -911,9 +1010,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B19">
         <v>13.09</v>
@@ -928,9 +1027,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <v>25.64</v>
@@ -945,9 +1044,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B21">
         <v>17.47</v>
@@ -960,6 +1059,713 @@
       </c>
       <c r="E21">
         <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>19.78</v>
+      </c>
+      <c r="C22">
+        <v>19.66</v>
+      </c>
+      <c r="D22">
+        <v>19.71</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>18.71</v>
+      </c>
+      <c r="C23">
+        <v>18.260000000000002</v>
+      </c>
+      <c r="D23">
+        <v>18.54</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>28.88</v>
+      </c>
+      <c r="C24">
+        <v>28.08</v>
+      </c>
+      <c r="D24">
+        <v>28.46</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>30.65</v>
+      </c>
+      <c r="G24">
+        <v>31.08</v>
+      </c>
+      <c r="H24">
+        <v>30.89</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>16.07</v>
+      </c>
+      <c r="C25">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="D25">
+        <v>16.21</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="G25">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="H25">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>18.09</v>
+      </c>
+      <c r="C26">
+        <v>18.190000000000001</v>
+      </c>
+      <c r="D26">
+        <v>18.13</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="G26">
+        <v>19.97</v>
+      </c>
+      <c r="H26">
+        <v>19.89</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>14.58</v>
+      </c>
+      <c r="C27">
+        <v>14.75</v>
+      </c>
+      <c r="D27">
+        <v>14.98</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>15.35</v>
+      </c>
+      <c r="G27">
+        <v>15.37</v>
+      </c>
+      <c r="H27">
+        <v>15.36</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>24.45</v>
+      </c>
+      <c r="C28">
+        <v>25.16</v>
+      </c>
+      <c r="D28">
+        <v>24.93</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>24.92</v>
+      </c>
+      <c r="C29">
+        <v>24.71</v>
+      </c>
+      <c r="D29">
+        <v>24.82</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="C30">
+        <v>16.2</v>
+      </c>
+      <c r="D30">
+        <v>16.21</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>14.33</v>
+      </c>
+      <c r="G30">
+        <v>14.83</v>
+      </c>
+      <c r="H30">
+        <v>14.56</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>23.75</v>
+      </c>
+      <c r="C31">
+        <v>23.69</v>
+      </c>
+      <c r="D31">
+        <v>23.72</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="C32">
+        <v>16.61</v>
+      </c>
+      <c r="D32">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>17.510000000000002</v>
+      </c>
+      <c r="C33">
+        <v>17.61</v>
+      </c>
+      <c r="D33">
+        <v>17.55</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>20.36</v>
+      </c>
+      <c r="G33">
+        <v>20.88</v>
+      </c>
+      <c r="H33">
+        <v>20.94</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>15.53</v>
+      </c>
+      <c r="C34">
+        <v>15.75</v>
+      </c>
+      <c r="D34">
+        <v>15.66</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>22.13</v>
+      </c>
+      <c r="C35">
+        <v>21.62</v>
+      </c>
+      <c r="D35">
+        <v>21.96</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>19.63</v>
+      </c>
+      <c r="G35">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="H35">
+        <v>19.75</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>17.21</v>
+      </c>
+      <c r="C36">
+        <v>16.91</v>
+      </c>
+      <c r="D36">
+        <v>17.03</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>18.93</v>
+      </c>
+      <c r="G36">
+        <v>18.62</v>
+      </c>
+      <c r="H36">
+        <v>18.78</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>20.39</v>
+      </c>
+      <c r="C37">
+        <v>20.12</v>
+      </c>
+      <c r="D37">
+        <v>20.27</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>21.63</v>
+      </c>
+      <c r="C38">
+        <v>22.01</v>
+      </c>
+      <c r="D38">
+        <v>21.86</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>18.88</v>
+      </c>
+      <c r="C39">
+        <v>18.53</v>
+      </c>
+      <c r="D39">
+        <v>18.71</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>25.75</v>
+      </c>
+      <c r="C40">
+        <v>25.86</v>
+      </c>
+      <c r="D40">
+        <v>25.81</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>24.08</v>
+      </c>
+      <c r="G40">
+        <v>24.19</v>
+      </c>
+      <c r="H40">
+        <v>24.13</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="C41">
+        <v>16.34</v>
+      </c>
+      <c r="D41">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>15.11</v>
+      </c>
+      <c r="G41">
+        <v>15.34</v>
+      </c>
+      <c r="H41">
+        <v>15.22</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>18.13</v>
+      </c>
+      <c r="C42">
+        <v>18.27</v>
+      </c>
+      <c r="D42">
+        <v>18.21</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>19.41</v>
+      </c>
+      <c r="G42">
+        <v>19.25</v>
+      </c>
+      <c r="H42">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>26.69</v>
+      </c>
+      <c r="C43">
+        <v>27.13</v>
+      </c>
+      <c r="D43">
+        <v>26.88</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>24.86</v>
+      </c>
+      <c r="G43">
+        <v>25.13</v>
+      </c>
+      <c r="H43">
+        <v>25.02</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>23.42</v>
+      </c>
+      <c r="C44">
+        <v>22.92</v>
+      </c>
+      <c r="D44">
+        <v>23.03</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>27.14</v>
+      </c>
+      <c r="C45">
+        <v>27.24</v>
+      </c>
+      <c r="D45">
+        <v>27.56</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>20.47</v>
+      </c>
+      <c r="C46">
+        <v>20.57</v>
+      </c>
+      <c r="D46">
+        <v>20.51</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>21.83</v>
+      </c>
+      <c r="G46">
+        <v>22.13</v>
+      </c>
+      <c r="H46">
+        <v>22.05</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>15.67</v>
+      </c>
+      <c r="C47">
+        <v>15.96</v>
+      </c>
+      <c r="D47">
+        <v>15.52</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>20.81</v>
+      </c>
+      <c r="C48">
+        <v>20.98</v>
+      </c>
+      <c r="D48">
+        <v>20.88</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>21.32</v>
+      </c>
+      <c r="G48">
+        <v>21.55</v>
+      </c>
+      <c r="H48">
+        <v>21.44</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>18.32</v>
+      </c>
+      <c r="C49">
+        <v>18.16</v>
+      </c>
+      <c r="D49">
+        <v>18.23</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>20.05</v>
+      </c>
+      <c r="G49">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="H49">
+        <v>20.07</v>
+      </c>
+      <c r="I49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>25.62</v>
+      </c>
+      <c r="C50">
+        <v>26.26</v>
+      </c>
+      <c r="D50">
+        <v>25.98</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>16.86</v>
+      </c>
+      <c r="C51">
+        <v>16.86</v>
+      </c>
+      <c r="D51">
+        <v>16.809999999999999</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>14.29</v>
+      </c>
+      <c r="C52">
+        <v>14.29</v>
+      </c>
+      <c r="D52">
+        <v>14.18</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>